<commit_message>
add TN List generator
</commit_message>
<xml_diff>
--- a/packages/app/public/templates/kueche.xlsx
+++ b/packages/app/public/templates/kueche.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\app\packages\app\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AECDA40-C0FF-4A6A-99F7-BEE0B133CF3B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811007B9-3405-4F70-A974-CD7A3E1BB71B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teilnehmerliste" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Teilnehmerliste!$1:$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Vorname</t>
   </si>
@@ -52,9 +51,6 @@
   </si>
   <si>
     <t>Nachname</t>
-  </si>
-  <si>
-    <t>Freizeitname</t>
   </si>
   <si>
     <t>Geburts-
@@ -64,9 +60,6 @@
     <t>Leiter:</t>
   </si>
   <si>
-    <t>Freizeitleiter</t>
-  </si>
-  <si>
     <t>Anmelde-ID</t>
   </si>
   <si>
@@ -110,6 +103,18 @@
   </si>
   <si>
     <t>${table:anmeldungen.email.eMail}</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>${begin.german}</t>
+  </si>
+  <si>
+    <t>${ende.german}</t>
+  </si>
+  <si>
+    <t>${bezeichnung}</t>
   </si>
 </sst>
 </file>
@@ -117,8 +122,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy&quot;  -  &quot;"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot;  -  &quot;"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -378,22 +383,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="27">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -401,26 +406,22 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,11 +430,11 @@
     <xf numFmtId="14" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -459,83 +460,19 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -943,7 +880,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -968,29 +905,29 @@
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1">
       <c r="D2" s="26" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17" t="s">
-        <v>8</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5">
-        <v>43288</v>
-      </c>
-      <c r="G3" s="6">
-        <v>43298</v>
+      <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="7.15" customHeight="1">
@@ -1000,67 +937,67 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="F6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>16</v>
+      <c r="J6" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="27.95" customHeight="1" thickTop="1">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="D7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="I7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="18" t="s">
+      <c r="J7" s="23" t="s">
         <v>22</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
@@ -1070,7 +1007,7 @@
       <c r="G17"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="27"/>
+      <c r="G18" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:AL7">

</xml_diff>

<commit_message>
some fixes hauptleiter in tnlisten
</commit_message>
<xml_diff>
--- a/packages/app/public/templates/kueche.xlsx
+++ b/packages/app/public/templates/kueche.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\app\packages\app\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\ec\ec-verwaltungs-app\packages\app\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B6B6F-3CD7-4EA6-987A-A03B34092DB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE60D99-C6E5-4CE1-AC4B-B5ACD20231B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Vorname</t>
   </si>
@@ -57,9 +57,6 @@
 datum</t>
   </si>
   <si>
-    <t>Leiter:</t>
-  </si>
-  <si>
     <t>${table:anmeldungen.person.nachname}</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>${table:anmeldungen.email.eMail}</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>${begin.german}</t>
   </si>
   <si>
@@ -115,6 +109,9 @@
   </si>
   <si>
     <t>Fortl.-ID</t>
+  </si>
+  <si>
+    <t>Leiter:  ${hauptleiter.person.vorname} ${hauptleiter.person.nachname}</t>
   </si>
 </sst>
 </file>
@@ -430,10 +427,6 @@
     <xf numFmtId="14" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -466,6 +459,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -874,13 +871,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -897,37 +894,35 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" customHeight="1">
       <c r="D1" s="2"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1">
-      <c r="D2" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="D2" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="C3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="26"/>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="7.15" customHeight="1">
@@ -938,7 +933,7 @@
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
       <c r="A6" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>5</v>
@@ -947,16 +942,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -965,57 +960,61 @@
         <v>1</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="27.95" customHeight="1" thickTop="1">
-      <c r="A7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="I7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="G16"/>
     </row>
-    <row r="17" spans="7:7" ht="15">
+    <row r="17" spans="5:7" ht="15">
       <c r="G17"/>
     </row>
-    <row r="18" spans="7:7">
-      <c r="G18" s="24"/>
+    <row r="18" spans="5:7">
+      <c r="G18" s="23"/>
+    </row>
+    <row r="26" spans="5:7">
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:AL7">
     <sortCondition ref="B7"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="D2:G2"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="82" fitToHeight="2" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>